<commit_message>
parameter read in working ok
</commit_message>
<xml_diff>
--- a/UserInputSheet.xlsx
+++ b/UserInputSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Dads Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D84F147-7F93-49D1-A4B0-9B6E5204AF39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F52F7E1-E99C-4BBB-96E8-52BD29796679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26205" yWindow="495" windowWidth="13830" windowHeight="7170" xr2:uid="{661BF5FC-8EDB-49B8-9F5E-EFC5E7050048}"/>
+    <workbookView xWindow="-12480" yWindow="1815" windowWidth="11070" windowHeight="5730" xr2:uid="{661BF5FC-8EDB-49B8-9F5E-EFC5E7050048}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="6" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="68">
   <si>
     <t>Brick</t>
   </si>
@@ -233,9 +233,6 @@
     <t>external material thickness (cm)</t>
   </si>
   <si>
-    <t>construction</t>
-  </si>
-  <si>
     <t>volume (m^3)</t>
   </si>
   <si>
@@ -260,9 +257,6 @@
     <t>Temperature Profile</t>
   </si>
   <si>
-    <t>Outside Temperature</t>
-  </si>
-  <si>
     <t>Target Temperature</t>
   </si>
   <si>
@@ -291,6 +285,18 @@
   </si>
   <si>
     <t>type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>Exterior Temperature</t>
+  </si>
+  <si>
+    <t>area to lower level (m^3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> area (m^2)</t>
   </si>
 </sst>
 </file>
@@ -768,7 +774,7 @@
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -794,23 +800,25 @@
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
       <c r="H1" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I1" s="21"/>
     </row>
     <row r="2" spans="1:9" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="12">
         <v>10</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="12" t="s">
+        <v>64</v>
+      </c>
       <c r="D2" s="13"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
       <c r="H2" s="7" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="I2" s="7">
         <v>10</v>
@@ -828,7 +836,7 @@
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
       <c r="H3" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I3" s="7">
         <v>18</v>
@@ -836,20 +844,20 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="10">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="13"/>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
       <c r="H4" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -891,8 +899,12 @@
       <c r="F7" s="10"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
+      <c r="A8" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="10">
+        <v>500</v>
+      </c>
       <c r="C8" s="10"/>
       <c r="D8" s="13"/>
       <c r="E8" s="10"/>
@@ -912,25 +924,25 @@
       </c>
       <c r="F9" s="8"/>
       <c r="H9" s="22" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I9" s="5"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="B10" s="10">
         <v>500</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="D10" s="13">
         <v>120</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="F10" s="10">
         <v>30</v>
@@ -950,7 +962,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F11" s="10" t="s">
         <v>21</v>
@@ -961,7 +973,7 @@
         <v>42</v>
       </c>
       <c r="B12" s="10">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>42</v>
@@ -970,10 +982,10 @@
         <v>5</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -1034,7 +1046,7 @@
     </row>
     <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A19" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B19" s="16"/>
       <c r="C19" s="9"/>
@@ -1044,7 +1056,7 @@
     </row>
     <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B20" s="12">
         <v>10</v>
@@ -1068,10 +1080,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B22" s="10">
-        <v>120</v>
+        <v>1200</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="13"/>
@@ -1115,8 +1127,12 @@
       <c r="F25" s="10"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
+      <c r="A26" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="10">
+        <v>500</v>
+      </c>
       <c r="C26" s="10"/>
       <c r="D26" s="13"/>
       <c r="E26" s="10"/>
@@ -1138,19 +1154,19 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="B28" s="10">
         <v>500</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="D28" s="13">
         <v>120</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="F28" s="10">
         <v>30</v>
@@ -1169,11 +1185,11 @@
       <c r="D29" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E29" s="10" t="s">
-        <v>46</v>
+      <c r="E29" s="23" t="s">
+        <v>62</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1189,8 +1205,12 @@
       <c r="D30" s="13">
         <v>5</v>
       </c>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
+      <c r="E30" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
@@ -1250,7 +1270,7 @@
     </row>
     <row r="37" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A37" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B37" s="18"/>
       <c r="C37" s="9"/>
@@ -1260,7 +1280,7 @@
     </row>
     <row r="38" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A38" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B38" s="12">
         <v>10</v>
@@ -1284,7 +1304,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B40" s="10">
         <v>1000</v>
@@ -1323,7 +1343,7 @@
         <v>40</v>
       </c>
       <c r="B43" s="10">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="13"/>
@@ -1331,8 +1351,12 @@
       <c r="F43" s="10"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" s="10"/>
-      <c r="B44" s="10"/>
+      <c r="A44" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B44" s="10">
+        <v>500</v>
+      </c>
       <c r="C44" s="10"/>
       <c r="D44" s="13"/>
       <c r="E44" s="10"/>
@@ -1344,13 +1368,13 @@
       </c>
       <c r="B45" s="18"/>
       <c r="C45" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="D45" s="18"/>
+        <v>34</v>
+      </c>
+      <c r="D45" s="19"/>
       <c r="E45" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="F45" s="19"/>
+        <v>51</v>
+      </c>
+      <c r="F45" s="18"/>
       <c r="G45" s="18" t="s">
         <v>35</v>
       </c>
@@ -1366,17 +1390,17 @@
       <c r="C46" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D46" s="10">
-        <v>500</v>
+      <c r="D46" s="13">
+        <v>120</v>
       </c>
       <c r="E46" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F46" s="13">
-        <v>120</v>
+      <c r="F46" s="10">
+        <v>500</v>
       </c>
       <c r="G46" s="10" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="H46" s="10">
         <v>30</v>
@@ -1393,19 +1417,19 @@
         <v>41</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E47" s="10" t="s">
         <v>41</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="G47" s="10" t="s">
-        <v>46</v>
+        <v>3</v>
+      </c>
+      <c r="G47" s="23" t="s">
+        <v>62</v>
       </c>
       <c r="H47" s="10" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
@@ -1413,22 +1437,26 @@
         <v>42</v>
       </c>
       <c r="B48" s="10">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C48" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D48" s="10">
-        <v>14</v>
+      <c r="D48" s="13">
+        <v>5</v>
       </c>
       <c r="E48" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="F48" s="13">
-        <v>5</v>
-      </c>
-      <c r="G48" s="10"/>
-      <c r="H48" s="10"/>
+      <c r="F48" s="10">
+        <v>15</v>
+      </c>
+      <c r="G48" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="H48" s="10" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="10" t="s">
@@ -1462,14 +1490,14 @@
       <c r="C50" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D50" s="10">
-        <v>0</v>
+      <c r="D50" s="13">
+        <v>175</v>
       </c>
       <c r="E50" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F50" s="13">
-        <v>175</v>
+      <c r="F50" s="10">
+        <v>0</v>
       </c>
       <c r="G50" s="10"/>
       <c r="H50" s="10"/>
@@ -1478,9 +1506,9 @@
       <c r="A51" s="10"/>
       <c r="B51" s="10"/>
       <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
+      <c r="D51" s="13"/>
       <c r="E51" s="10"/>
-      <c r="F51" s="13"/>
+      <c r="F51" s="10"/>
       <c r="G51" s="10"/>
       <c r="H51" s="10"/>
     </row>
@@ -1488,9 +1516,9 @@
       <c r="A52" s="10"/>
       <c r="B52" s="10"/>
       <c r="C52" s="10"/>
-      <c r="D52" s="10"/>
+      <c r="D52" s="13"/>
       <c r="E52" s="10"/>
-      <c r="F52" s="13"/>
+      <c r="F52" s="10"/>
       <c r="G52" s="10"/>
       <c r="H52" s="10"/>
     </row>
@@ -1498,9 +1526,9 @@
       <c r="A53" s="1"/>
       <c r="B53" s="10"/>
       <c r="C53" s="1"/>
-      <c r="D53" s="10"/>
+      <c r="D53" s="13"/>
       <c r="E53" s="1"/>
-      <c r="F53" s="13"/>
+      <c r="F53" s="10"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
     </row>
@@ -1513,13 +1541,13 @@
           <x14:formula1>
             <xm:f>Materials!$A$3:$A$16</xm:f>
           </x14:formula1>
-          <xm:sqref>B11 B13 D11 D13 B29 B31 D29 D31 F47 F49 B49 B47 D49 D47 F11</xm:sqref>
+          <xm:sqref>B11 B13 D11 D13 B29 B31 D29 D31 D47 D49 B49 B47 F11 F49 F47 F29 H47</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1C51B279-9347-4C56-8D0A-6867D59CEC48}">
           <x14:formula1>
             <xm:f>Materials!$A$20:$A$21</xm:f>
           </x14:formula1>
-          <xm:sqref>F12 F29 H47</xm:sqref>
+          <xm:sqref>F12 F30 H48</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1532,14 +1560,14 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>12</v>
@@ -1551,10 +1579,10 @@
         <v>14</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -1574,7 +1602,7 @@
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>19</v>
@@ -1950,12 +1978,12 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix bug with thickness
</commit_message>
<xml_diff>
--- a/UserInputSheet.xlsx
+++ b/UserInputSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Dads Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\.shortcut-targets-by-id\1-9BdNIiT7Zve61xm0MKrEiBMif4tQ21K\Dads Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F52F7E1-E99C-4BBB-96E8-52BD29796679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D723E5-1055-4157-9C17-1B6AA237B387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12480" yWindow="1815" windowWidth="11070" windowHeight="5730" xr2:uid="{661BF5FC-8EDB-49B8-9F5E-EFC5E7050048}"/>
+    <workbookView xWindow="13290" yWindow="90" windowWidth="15375" windowHeight="14850" xr2:uid="{661BF5FC-8EDB-49B8-9F5E-EFC5E7050048}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="6" r:id="rId1"/>
@@ -24,9 +24,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="67">
   <si>
     <t>Brick</t>
   </si>
@@ -227,9 +230,6 @@
     <t>external material type</t>
   </si>
   <si>
-    <t xml:space="preserve"> area (m^3)</t>
-  </si>
-  <si>
     <t>external material thickness (cm)</t>
   </si>
   <si>
@@ -260,9 +260,6 @@
     <t>Target Temperature</t>
   </si>
   <si>
-    <t>Middle</t>
-  </si>
-  <si>
     <t>ROUND THICKNESSES TO NEAREST 5CM!!</t>
   </si>
   <si>
@@ -297,6 +294,9 @@
   </si>
   <si>
     <t xml:space="preserve"> area (m^2)</t>
+  </si>
+  <si>
+    <t>Lower</t>
   </si>
 </sst>
 </file>
@@ -426,7 +426,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -440,12 +440,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -773,762 +771,760 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{776440E9-42E3-4F35-BD1F-E92FBB255ADE}">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" style="11" customWidth="1"/>
-    <col min="3" max="3" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="14" customWidth="1"/>
-    <col min="5" max="5" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" style="7"/>
+    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:9" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="H1" s="20" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="H1" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="19"/>
+    </row>
+    <row r="2" spans="1:9" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="9">
+        <v>5</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="11"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="H2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="9">
+        <v>38000</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="H3" t="s">
         <v>53</v>
       </c>
-      <c r="I1" s="21"/>
-    </row>
-    <row r="2" spans="1:9" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="I3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1000</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="H4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="9">
+        <v>1206</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="9">
+        <v>20</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="9">
+        <v>500</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="1:9" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="H9" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="9">
+        <v>500</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="11">
+        <v>120</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="9">
+        <v>5</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="11">
+        <v>17.5</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="12">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="H2" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="I2" s="7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="10">
-        <v>38000</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="H3" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="I3" s="7">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="10">
-        <v>1000</v>
-      </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="H4" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="10">
-        <v>1206</v>
-      </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="H5" s="7"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="10">
-        <v>20</v>
-      </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="H6" s="7"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B8" s="10">
-        <v>500</v>
-      </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-    </row>
-    <row r="9" spans="1:9" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" s="8"/>
-      <c r="H9" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="I9" s="5"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="10">
-        <v>500</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" s="13">
-        <v>120</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="F10" s="10">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" s="10">
-        <v>20</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="13">
-        <v>5</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
+      <c r="C13" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="10">
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="9">
         <v>0</v>
       </c>
-      <c r="C14" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="13">
-        <v>175</v>
-      </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C14" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="11">
+        <v>0</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="10"/>
+      <c r="B17" s="9"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="13"/>
+      <c r="D17" s="11"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A19" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-    </row>
-    <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A20" s="12" t="s">
+    <row r="19" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="14"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+    </row>
+    <row r="20" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="9">
+        <v>5</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="9">
+        <v>0</v>
+      </c>
+      <c r="C21" s="9"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="9">
+        <v>1000</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="9">
+        <v>1206</v>
+      </c>
+      <c r="C23" s="9"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="9">
+        <v>20</v>
+      </c>
+      <c r="C24" s="9"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="C25" s="9"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="9">
+        <v>500</v>
+      </c>
+      <c r="C26" s="9"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A27" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="15"/>
+      <c r="E27" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F27" s="14"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" s="11">
+        <v>120</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F28" s="9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="9">
+        <v>15</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" s="11">
+        <v>17.5</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F30" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="12">
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="10">
-        <v>38000</v>
-      </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" s="10">
-        <v>1200</v>
-      </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" s="10">
-        <v>1206</v>
-      </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="10">
-        <v>20</v>
-      </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="C25" s="10"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="B26" s="10">
-        <v>500</v>
-      </c>
-      <c r="C26" s="10"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-    </row>
-    <row r="27" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A27" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D27" s="17"/>
-      <c r="E27" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="F27" s="16"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B28" s="10">
-        <v>500</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D28" s="13">
-        <v>120</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="F28" s="10">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E29" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="F29" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B30" s="10">
-        <v>15</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D30" s="13">
-        <v>5</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="10" t="s">
+      <c r="C31" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D31" s="10" t="s">
+      <c r="D31" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B32" s="10">
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="9">
         <v>0</v>
       </c>
-      <c r="C32" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D32" s="13">
-        <v>175</v>
-      </c>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="10"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="10"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C32" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" s="11">
+        <v>0</v>
+      </c>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
-      <c r="B35" s="10"/>
+      <c r="B35" s="9"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="13"/>
+      <c r="D35" s="11"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
     </row>
-    <row r="37" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A37" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B37" s="18"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-    </row>
-    <row r="38" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A38" s="12" t="s">
+    <row r="37" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A37" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="16"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+    </row>
+    <row r="38" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A38" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" s="9">
+        <v>5</v>
+      </c>
+      <c r="C38" s="9"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="9">
+        <v>0</v>
+      </c>
+      <c r="C39" s="9"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" s="9">
+        <v>1000</v>
+      </c>
+      <c r="C40" s="9"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" s="9">
+        <v>1206</v>
+      </c>
+      <c r="C41" s="9"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42" s="9">
+        <v>0</v>
+      </c>
+      <c r="C42" s="9"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="C43" s="9"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B44" s="9">
+        <v>500</v>
+      </c>
+      <c r="C44" s="9"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+    </row>
+    <row r="45" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A45" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B45" s="16"/>
+      <c r="C45" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D45" s="17"/>
+      <c r="E45" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H45" s="16"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B46" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D46" s="11">
+        <v>120</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F46" s="9">
+        <v>500</v>
+      </c>
+      <c r="G46" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="H46" s="9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G47" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="H47" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B48" s="9">
+        <v>15</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D48" s="11">
+        <v>17.5</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F48" s="9">
+        <v>5</v>
+      </c>
+      <c r="G48" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="H48" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B38" s="12">
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B49" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C38" s="12"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39" s="10">
-        <v>38000</v>
-      </c>
-      <c r="C39" s="10"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B40" s="10">
-        <v>1000</v>
-      </c>
-      <c r="C40" s="10"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B41" s="10">
-        <v>1206</v>
-      </c>
-      <c r="C41" s="10"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B42" s="10">
+      <c r="C49" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D49" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="10"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B43" s="10">
-        <v>2</v>
-      </c>
-      <c r="C43" s="10"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B44" s="10">
-        <v>500</v>
-      </c>
-      <c r="C44" s="10"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="10"/>
-    </row>
-    <row r="45" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A45" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D45" s="19"/>
-      <c r="E45" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="F45" s="18"/>
-      <c r="G45" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="H45" s="18"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" s="10" t="s">
+      <c r="E49" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G49" s="9"/>
+      <c r="H49" s="9"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B46" s="10">
-        <v>500</v>
-      </c>
-      <c r="C46" s="10" t="s">
+      <c r="B50" s="9">
+        <v>0</v>
+      </c>
+      <c r="C50" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D46" s="13">
-        <v>120</v>
-      </c>
-      <c r="E46" s="10" t="s">
+      <c r="D50" s="11">
+        <v>0</v>
+      </c>
+      <c r="E50" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F46" s="10">
-        <v>500</v>
-      </c>
-      <c r="G46" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="H46" s="10">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A47" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B47" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C47" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D47" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E47" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="F47" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G47" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="H47" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A48" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B48" s="10">
-        <v>15</v>
-      </c>
-      <c r="C48" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D48" s="13">
-        <v>5</v>
-      </c>
-      <c r="E48" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="F48" s="10">
-        <v>15</v>
-      </c>
-      <c r="G48" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="H48" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A49" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B49" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C49" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D49" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="E49" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F49" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="G49" s="10"/>
-      <c r="H49" s="10"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A50" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B50" s="10">
-        <v>0</v>
-      </c>
-      <c r="C50" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D50" s="13">
-        <v>175</v>
-      </c>
-      <c r="E50" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F50" s="10">
-        <v>0</v>
-      </c>
-      <c r="G50" s="10"/>
-      <c r="H50" s="10"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A51" s="10"/>
-      <c r="B51" s="10"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="13"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="10"/>
-      <c r="G51" s="10"/>
-      <c r="H51" s="10"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A52" s="10"/>
-      <c r="B52" s="10"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="10"/>
-      <c r="F52" s="10"/>
-      <c r="G52" s="10"/>
-      <c r="H52" s="10"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F50" s="9">
+        <v>50</v>
+      </c>
+      <c r="G50" s="9"/>
+      <c r="H50" s="9"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="9"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="9"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="9"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="9"/>
+      <c r="H52" s="9"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
-      <c r="B53" s="10"/>
+      <c r="B53" s="9"/>
       <c r="C53" s="1"/>
-      <c r="D53" s="13"/>
+      <c r="D53" s="11"/>
       <c r="E53" s="1"/>
-      <c r="F53" s="10"/>
+      <c r="F53" s="9"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
     </row>
@@ -1563,11 +1559,11 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>12</v>
@@ -1579,13 +1575,13 @@
         <v>14</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>8</v>
@@ -1602,13 +1598,13 @@
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1635,7 +1631,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1662,7 +1658,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1686,7 +1682,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1713,7 +1709,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -1740,7 +1736,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1767,7 +1763,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1794,7 +1790,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1820,7 +1816,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1847,7 +1843,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1871,7 +1867,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1898,7 +1894,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1925,7 +1921,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1952,7 +1948,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1976,14 +1972,14 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add radiant heat to surfaces
</commit_message>
<xml_diff>
--- a/UserInputSheet.xlsx
+++ b/UserInputSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\.shortcut-targets-by-id\1-9BdNIiT7Zve61xm0MKrEiBMif4tQ21K\Dads Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Dads Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D723E5-1055-4157-9C17-1B6AA237B387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7411249-1475-405D-B7B2-E1FB6D410D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13290" yWindow="90" windowWidth="15375" windowHeight="14850" xr2:uid="{661BF5FC-8EDB-49B8-9F5E-EFC5E7050048}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{661BF5FC-8EDB-49B8-9F5E-EFC5E7050048}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="6" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="70">
   <si>
     <t>Brick</t>
   </si>
@@ -260,9 +260,6 @@
     <t>Target Temperature</t>
   </si>
   <si>
-    <t>ROUND THICKNESSES TO NEAREST 5CM!!</t>
-  </si>
-  <si>
     <t>Target Level</t>
   </si>
   <si>
@@ -297,6 +294,18 @@
   </si>
   <si>
     <t>Lower</t>
+  </si>
+  <si>
+    <t>ROUND THICKNESSES TO NEAREST 0.5CM!!</t>
+  </si>
+  <si>
+    <t>Radiant Heat in (W)</t>
+  </si>
+  <si>
+    <t># not used for now</t>
+  </si>
+  <si>
+    <t>DO NOT CHANGE LAYOUT</t>
   </si>
 </sst>
 </file>
@@ -426,7 +435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -455,6 +464,7 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -769,26 +779,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{776440E9-42E3-4F35-BD1F-E92FBB255ADE}">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875"/>
+    <col min="1" max="1" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="12" customWidth="1"/>
+    <col min="5" max="5" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>36</v>
       </c>
@@ -802,27 +811,27 @@
       </c>
       <c r="I1" s="19"/>
     </row>
-    <row r="2" spans="1:9" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>46</v>
       </c>
       <c r="B2" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="H2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>37</v>
       </c>
@@ -837,10 +846,10 @@
         <v>53</v>
       </c>
       <c r="I3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>45</v>
       </c>
@@ -852,13 +861,16 @@
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="H4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="J4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>38</v>
       </c>
@@ -870,7 +882,7 @@
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>39</v>
       </c>
@@ -882,7 +894,7 @@
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>40</v>
       </c>
@@ -894,9 +906,9 @@
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B8" s="9">
         <v>500</v>
@@ -906,7 +918,7 @@
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
     </row>
-    <row r="9" spans="1:9" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>33</v>
       </c>
@@ -920,31 +932,34 @@
       </c>
       <c r="F9" s="7"/>
       <c r="H9" s="20" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="I9" s="5"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B10" s="9">
         <v>500</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D10" s="11">
         <v>120</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F10" s="9">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H10" s="22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>41</v>
       </c>
@@ -955,21 +970,21 @@
         <v>41</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>42</v>
       </c>
       <c r="B12" s="9">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>42</v>
@@ -978,13 +993,13 @@
         <v>17.5</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>43</v>
       </c>
@@ -997,10 +1012,14 @@
       <c r="D13" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E13" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>44</v>
       </c>
@@ -1016,15 +1035,23 @@
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="11"/>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="9">
+        <v>0</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="9">
+        <v>0</v>
+      </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -1032,7 +1059,7 @@
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="9"/>
       <c r="C17" s="1"/>
@@ -1040,7 +1067,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="19" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A19" s="14" t="s">
         <v>49</v>
       </c>
@@ -1050,19 +1077,19 @@
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
         <v>46</v>
       </c>
       <c r="B20" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="11"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>37</v>
       </c>
@@ -1074,7 +1101,7 @@
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>45</v>
       </c>
@@ -1086,7 +1113,7 @@
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
         <v>38</v>
       </c>
@@ -1098,7 +1125,7 @@
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
         <v>39</v>
       </c>
@@ -1110,7 +1137,7 @@
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>40</v>
       </c>
@@ -1122,9 +1149,9 @@
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B26" s="9">
         <v>500</v>
@@ -1134,7 +1161,7 @@
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
     </row>
-    <row r="27" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A27" s="14" t="s">
         <v>33</v>
       </c>
@@ -1148,27 +1175,27 @@
       </c>
       <c r="F27" s="14"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B28" s="9">
         <v>1E-3</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D28" s="11">
         <v>120</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F28" s="9">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>41</v>
       </c>
@@ -1179,16 +1206,16 @@
         <v>41</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F29" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
         <v>42</v>
       </c>
@@ -1202,13 +1229,13 @@
         <v>17.5</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F30" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
         <v>43</v>
       </c>
@@ -1221,10 +1248,14 @@
       <c r="D31" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E31" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F31" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
         <v>44</v>
       </c>
@@ -1240,15 +1271,23 @@
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="9"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="11"/>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" s="9">
+        <v>0</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" s="9">
+        <v>0</v>
+      </c>
       <c r="E33" s="9"/>
       <c r="F33" s="9"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="9"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
@@ -1256,7 +1295,7 @@
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="9"/>
       <c r="C35" s="1"/>
@@ -1264,7 +1303,7 @@
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
     </row>
-    <row r="37" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A37" s="16" t="s">
         <v>51</v>
       </c>
@@ -1274,19 +1313,19 @@
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
     </row>
-    <row r="38" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
         <v>46</v>
       </c>
       <c r="B38" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C38" s="9"/>
       <c r="D38" s="11"/>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
         <v>37</v>
       </c>
@@ -1298,7 +1337,7 @@
       <c r="E39" s="9"/>
       <c r="F39" s="9"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
         <v>45</v>
       </c>
@@ -1310,7 +1349,7 @@
       <c r="E40" s="9"/>
       <c r="F40" s="9"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
         <v>38</v>
       </c>
@@ -1322,7 +1361,7 @@
       <c r="E41" s="9"/>
       <c r="F41" s="9"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
         <v>39</v>
       </c>
@@ -1334,7 +1373,7 @@
       <c r="E42" s="9"/>
       <c r="F42" s="9"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
         <v>40</v>
       </c>
@@ -1346,9 +1385,9 @@
       <c r="E43" s="9"/>
       <c r="F43" s="9"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B44" s="9">
         <v>500</v>
@@ -1358,7 +1397,7 @@
       <c r="E44" s="9"/>
       <c r="F44" s="9"/>
     </row>
-    <row r="45" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A45" s="16" t="s">
         <v>33</v>
       </c>
@@ -1376,33 +1415,33 @@
       </c>
       <c r="H45" s="16"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B46" s="9">
         <v>1E-3</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D46" s="11">
         <v>120</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F46" s="9">
         <v>500</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H46" s="9">
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
         <v>41</v>
       </c>
@@ -1422,13 +1461,13 @@
         <v>9</v>
       </c>
       <c r="G47" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H47" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
         <v>42</v>
       </c>
@@ -1448,13 +1487,13 @@
         <v>5</v>
       </c>
       <c r="G48" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H48" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="9" t="s">
         <v>43</v>
       </c>
@@ -1473,10 +1512,14 @@
       <c r="F49" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G49" s="9"/>
-      <c r="H49" s="9"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G49" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="H49" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="s">
         <v>44</v>
       </c>
@@ -1498,17 +1541,29 @@
       <c r="G50" s="9"/>
       <c r="H50" s="9"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="9"/>
-      <c r="B51" s="9"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="9"/>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B51" s="9">
+        <v>0</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D51" s="9">
+        <v>10000</v>
+      </c>
+      <c r="E51" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F51" s="9">
+        <v>0</v>
+      </c>
       <c r="G51" s="9"/>
       <c r="H51" s="9"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="9"/>
       <c r="B52" s="9"/>
       <c r="C52" s="9"/>
@@ -1518,7 +1573,7 @@
       <c r="G52" s="9"/>
       <c r="H52" s="9"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="9"/>
       <c r="C53" s="1"/>
@@ -1530,6 +1585,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -1559,11 +1615,11 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>12</v>
@@ -1575,13 +1631,13 @@
         <v>14</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>8</v>
@@ -1598,13 +1654,13 @@
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1631,7 +1687,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1658,7 +1714,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1682,7 +1738,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1709,7 +1765,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -1736,7 +1792,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1763,7 +1819,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1790,7 +1846,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1816,7 +1872,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1843,7 +1899,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1867,7 +1923,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1894,7 +1950,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1921,7 +1977,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1948,7 +2004,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1972,12 +2028,12 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
add progress bar, add hot spots, add modualted Qrad)
</commit_message>
<xml_diff>
--- a/UserInputSheet.xlsx
+++ b/UserInputSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Dads Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1151B7-02CD-44C7-9F40-EBD87BB0A838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB555FA-182F-4498-91D4-6866F3A2309E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{661BF5FC-8EDB-49B8-9F5E-EFC5E7050048}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="77">
   <si>
     <t>Brick</t>
   </si>
@@ -270,9 +270,6 @@
     <t>type</t>
   </si>
   <si>
-    <t xml:space="preserve">  </t>
-  </si>
-  <si>
     <t>Exterior Temperature</t>
   </si>
   <si>
@@ -307,6 +304,18 @@
   </si>
   <si>
     <t>thicnkess</t>
+  </si>
+  <si>
+    <t>Internals</t>
+  </si>
+  <si>
+    <t>Hot Spot</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>volume</t>
   </si>
 </sst>
 </file>
@@ -806,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{776440E9-42E3-4F35-BD1F-E92FBB255ADE}">
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38:F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -817,7 +826,7 @@
     <col min="3" max="3" width="29.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5546875" style="12" customWidth="1"/>
     <col min="5" max="5" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24.44140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -827,10 +836,10 @@
         <v>36</v>
       </c>
       <c r="B1" s="7"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
       <c r="H1" s="18" t="s">
         <v>52</v>
       </c>
@@ -843,14 +852,16 @@
       <c r="B2" s="9">
         <v>0</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>61</v>
+      <c r="C2" s="8" t="s">
+        <v>73</v>
       </c>
       <c r="D2" s="11"/>
-      <c r="E2" s="8"/>
+      <c r="E2" s="8" t="s">
+        <v>74</v>
+      </c>
       <c r="F2" s="8"/>
       <c r="H2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -863,10 +874,18 @@
       <c r="B3" s="9">
         <v>0</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
+      <c r="C3" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="11">
+        <v>100</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="9">
+        <v>5</v>
+      </c>
       <c r="H3" t="s">
         <v>53</v>
       </c>
@@ -881,18 +900,26 @@
       <c r="B4" s="9">
         <v>1000</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="C4" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="11">
+        <v>100</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="H4" t="s">
         <v>54</v>
       </c>
       <c r="I4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -902,10 +929,18 @@
       <c r="B5" s="9">
         <v>1206</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="C5" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="9">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
@@ -916,8 +951,12 @@
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="11"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
+      <c r="E6" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
@@ -928,20 +967,28 @@
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="11"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
+      <c r="E7" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B8" s="9">
         <v>500</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="11"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
+      <c r="E8" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:10" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
@@ -957,31 +1004,31 @@
       </c>
       <c r="F9" s="7"/>
       <c r="H9" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B10" s="9">
         <v>500</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D10" s="11">
         <v>225</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F10" s="9">
         <v>30</v>
       </c>
       <c r="H10" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -1038,7 +1085,7 @@
         <v>0</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F13" s="9">
         <v>0</v>
@@ -1058,7 +1105,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F14" s="9">
         <v>1</v>
@@ -1066,13 +1113,13 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B15" s="9">
         <v>0</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D15" s="9">
         <v>0</v>
@@ -1101,10 +1148,6 @@
         <v>49</v>
       </c>
       <c r="B19" s="14"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
     </row>
     <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
@@ -1113,9 +1156,13 @@
       <c r="B20" s="9">
         <v>0</v>
       </c>
-      <c r="C20" s="9"/>
+      <c r="C20" s="8" t="s">
+        <v>73</v>
+      </c>
       <c r="D20" s="11"/>
-      <c r="E20" s="8"/>
+      <c r="E20" s="8" t="s">
+        <v>74</v>
+      </c>
       <c r="F20" s="8"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1125,10 +1172,18 @@
       <c r="B21" s="9">
         <v>0</v>
       </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
+      <c r="C21" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="11">
+        <v>100</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21" s="9">
+        <v>5</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
@@ -1137,10 +1192,18 @@
       <c r="B22" s="9">
         <v>1000</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
+      <c r="C22" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="11">
+        <v>100</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
@@ -1149,10 +1212,18 @@
       <c r="B23" s="9">
         <v>1206</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
+      <c r="C23" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" s="9">
+        <v>10</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
@@ -1163,8 +1234,12 @@
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="11"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
+      <c r="E24" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
@@ -1175,20 +1250,28 @@
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="11"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
+      <c r="E25" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B26" s="9">
         <v>500</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="11"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
+      <c r="E26" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A27" s="14" t="s">
@@ -1206,19 +1289,19 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B28" s="9">
         <v>1E-3</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D28" s="11">
         <v>225</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F28" s="9">
         <v>30</v>
@@ -1278,7 +1361,7 @@
         <v>0</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F31" s="9">
         <v>0</v>
@@ -1298,7 +1381,7 @@
         <v>0</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F32" s="9">
         <v>1</v>
@@ -1306,13 +1389,13 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B33" s="9">
         <v>0</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D33" s="9">
         <v>22000</v>
@@ -1341,10 +1424,6 @@
         <v>51</v>
       </c>
       <c r="B37" s="16"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
     </row>
     <row r="38" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
@@ -1353,9 +1432,13 @@
       <c r="B38" s="9">
         <v>0</v>
       </c>
-      <c r="C38" s="9"/>
+      <c r="C38" s="8" t="s">
+        <v>73</v>
+      </c>
       <c r="D38" s="11"/>
-      <c r="E38" s="8"/>
+      <c r="E38" s="8" t="s">
+        <v>74</v>
+      </c>
       <c r="F38" s="8"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -1365,10 +1448,18 @@
       <c r="B39" s="9">
         <v>55579.3</v>
       </c>
-      <c r="C39" s="9"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
+      <c r="C39" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D39" s="11">
+        <v>100</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F39" s="9">
+        <v>5</v>
+      </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
@@ -1377,10 +1468,18 @@
       <c r="B40" s="9">
         <v>1000</v>
       </c>
-      <c r="C40" s="9"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
+      <c r="C40" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D40" s="11">
+        <v>100</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
@@ -1389,10 +1488,18 @@
       <c r="B41" s="9">
         <v>1206</v>
       </c>
-      <c r="C41" s="9"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
+      <c r="C41" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F41" s="9">
+        <v>10</v>
+      </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
@@ -1403,8 +1510,12 @@
       </c>
       <c r="C42" s="9"/>
       <c r="D42" s="11"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
+      <c r="E42" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
@@ -1415,20 +1526,28 @@
       </c>
       <c r="C43" s="9"/>
       <c r="D43" s="11"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
+      <c r="E43" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F43" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B44" s="9">
         <v>500</v>
       </c>
       <c r="C44" s="9"/>
       <c r="D44" s="11"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
+      <c r="E44" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="F44" s="9">
+        <v>1000</v>
+      </c>
     </row>
     <row r="45" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A45" s="16" t="s">
@@ -1450,25 +1569,25 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B46" s="9">
         <v>1E-3</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D46" s="11">
         <v>220</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F46" s="9">
         <v>500</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H46" s="9">
         <v>30</v>
@@ -1546,7 +1665,7 @@
         <v>9</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H49" s="9">
         <v>0</v>
@@ -1572,7 +1691,7 @@
         <v>50</v>
       </c>
       <c r="G50" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H50" s="9">
         <v>1</v>
@@ -1580,19 +1699,19 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B51" s="9">
         <v>0</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D51" s="9">
         <v>0</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F51" s="9">
         <v>0</v>
@@ -1630,7 +1749,7 @@
           <x14:formula1>
             <xm:f>Materials!$A$3:$A$17</xm:f>
           </x14:formula1>
-          <xm:sqref>B11 B13 D11 D13 B29 B31 D29 D31 D47 D49 B49 B47 F11 F49 F47 F29 H47</xm:sqref>
+          <xm:sqref>B11 B13 D11 D13 B29 B31 D29 D31 D47 D49 B49 B47 F11 F49 F47 F29 H47 F4 F6 D41 F22 F24 D23 F40 F42 D5</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1C51B279-9347-4C56-8D0A-6867D59CEC48}">
           <x14:formula1>
@@ -2072,7 +2191,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B17" s="4">
         <v>15</v>
@@ -2094,7 +2213,7 @@
         <v>6.4</v>
       </c>
       <c r="I17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
hotspot and internals working ok
</commit_message>
<xml_diff>
--- a/UserInputSheet.xlsx
+++ b/UserInputSheet.xlsx
@@ -5,40 +5,29 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\.shortcut-targets-by-id\1-9BdNIiT7Zve61xm0MKrEiBMif4tQ21K\Dads Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Dads Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39604796-B5E7-437B-8E57-3A9D8598306C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B94A14A-C047-46A8-AFC8-7C759D199F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{661BF5FC-8EDB-49B8-9F5E-EFC5E7050048}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{661BF5FC-8EDB-49B8-9F5E-EFC5E7050048}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="6" r:id="rId1"/>
     <sheet name="Materials" sheetId="7" r:id="rId2"/>
-    <sheet name="Boiler radiator model" sheetId="8" r:id="rId3"/>
+    <sheet name="Heat generator system model" sheetId="8" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" iterate="1" iterateCount="200" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="112">
   <si>
     <t>Brick</t>
   </si>
@@ -324,18 +313,9 @@
     <t>Hot Spot</t>
   </si>
   <si>
-    <t>area</t>
-  </si>
-  <si>
-    <t>volume</t>
-  </si>
-  <si>
     <t>Boiler efficiency</t>
   </si>
   <si>
-    <t>Boiler type</t>
-  </si>
-  <si>
     <t>condensing</t>
   </si>
   <si>
@@ -360,24 +340,9 @@
     <t>kg/m3</t>
   </si>
   <si>
-    <t>Number of radiators</t>
-  </si>
-  <si>
     <t>Length of pipework (m)</t>
   </si>
   <si>
-    <t>Per Radiator water volume (m3)</t>
-  </si>
-  <si>
-    <t>Per Radiator mass of steel (kg)</t>
-  </si>
-  <si>
-    <t>Radiator convective surface area (m2)</t>
-  </si>
-  <si>
-    <t>Radiator visible external surface area (m2)</t>
-  </si>
-  <si>
     <t>Pipework outside diameter (mm)</t>
   </si>
   <si>
@@ -405,9 +370,6 @@
     <t>Steel thermal inertia</t>
   </si>
   <si>
-    <t>Gas energy in to boiler (kW)</t>
-  </si>
-  <si>
     <t>Rate of temperature rise (no heat loss)</t>
   </si>
   <si>
@@ -424,14 +386,51 @@
   </si>
   <si>
     <t>but heat loss as it warm up will increase this time!!!</t>
+  </si>
+  <si>
+    <t>Energy in to boiler (kW)</t>
+  </si>
+  <si>
+    <t>Total thermal inertia</t>
+  </si>
+  <si>
+    <t>Radiator water volume (@0.008m3/kW)</t>
+  </si>
+  <si>
+    <t>Radiator mass @47kg/kW</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>water mass</t>
+  </si>
+  <si>
+    <t>Steel mass</t>
+  </si>
+  <si>
+    <t>Heat generator type</t>
+  </si>
+  <si>
+    <t>air to water heat pump</t>
+  </si>
+  <si>
+    <t>ground source heat pump</t>
+  </si>
+  <si>
+    <t>temperature</t>
+  </si>
+  <si>
+    <t>AREA MUST NOT BE ZERO AS CAUSES ERROR -&gt; MAKE V SMALL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0\ \C"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0\ \C"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -514,7 +513,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -551,8 +550,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -586,11 +591,73 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -629,19 +696,23 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -958,23 +1029,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{776440E9-42E3-4F35-BD1F-E92FBB255ADE}">
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="12" customWidth="1"/>
+    <col min="5" max="5" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>36</v>
       </c>
@@ -988,7 +1059,7 @@
       </c>
       <c r="I1" s="19"/>
     </row>
-    <row r="2" spans="1:10" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>46</v>
       </c>
@@ -1010,7 +1081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>37</v>
       </c>
@@ -1018,16 +1089,16 @@
         <v>0</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="D3" s="11">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>63</v>
       </c>
       <c r="F3" s="9">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="H3" t="s">
         <v>53</v>
@@ -1036,7 +1107,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>45</v>
       </c>
@@ -1044,10 +1115,10 @@
         <v>1000</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D4" s="11">
-        <v>1</v>
+        <v>41</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>0</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>41</v>
@@ -1065,7 +1136,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>38</v>
       </c>
@@ -1073,35 +1144,35 @@
         <v>1206</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>11</v>
+        <v>42</v>
+      </c>
+      <c r="D5" s="11">
+        <v>5.5</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>42</v>
+        <v>110</v>
       </c>
       <c r="F5" s="9">
-        <v>17.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>39</v>
       </c>
       <c r="B6" s="9">
         <v>20</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C6" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>40</v>
       </c>
@@ -1110,14 +1181,10 @@
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="11"/>
-      <c r="E7" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F7" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>63</v>
       </c>
@@ -1126,14 +1193,10 @@
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="11"/>
-      <c r="E8" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="F8" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="1:10" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>33</v>
       </c>
@@ -1151,7 +1214,7 @@
       </c>
       <c r="I9" s="5"/>
     </row>
-    <row r="10" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>63</v>
       </c>
@@ -1174,7 +1237,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>41</v>
       </c>
@@ -1193,8 +1256,11 @@
       <c r="F11" s="9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H11" s="22" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>42</v>
       </c>
@@ -1214,7 +1280,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>43</v>
       </c>
@@ -1234,7 +1300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>44</v>
       </c>
@@ -1254,7 +1320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>66</v>
       </c>
@@ -1270,7 +1336,7 @@
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -1278,7 +1344,7 @@
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="9"/>
       <c r="C17" s="1"/>
@@ -1286,13 +1352,13 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="19" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A19" s="14" t="s">
         <v>49</v>
       </c>
       <c r="B19" s="14"/>
     </row>
-    <row r="20" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
         <v>46</v>
       </c>
@@ -1308,7 +1374,7 @@
       </c>
       <c r="F20" s="8"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>37</v>
       </c>
@@ -1316,10 +1382,10 @@
         <v>0</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="D21" s="11">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>63</v>
@@ -1328,7 +1394,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>45</v>
       </c>
@@ -1336,10 +1402,10 @@
         <v>1000</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D22" s="11">
-        <v>10</v>
+        <v>41</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>0</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>41</v>
@@ -1348,7 +1414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
         <v>38</v>
       </c>
@@ -1356,35 +1422,35 @@
         <v>1206</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>9</v>
+        <v>42</v>
+      </c>
+      <c r="D23" s="11">
+        <v>17.5</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>42</v>
+        <v>110</v>
       </c>
       <c r="F23" s="9">
-        <v>17.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
         <v>39</v>
       </c>
       <c r="B24" s="9">
         <v>20</v>
       </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C24" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="9">
+        <v>0</v>
+      </c>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>40</v>
       </c>
@@ -1393,14 +1459,10 @@
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="11"/>
-      <c r="E25" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F25" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
         <v>62</v>
       </c>
@@ -1409,14 +1471,10 @@
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="11"/>
-      <c r="E26" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="F26" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A27" s="14" t="s">
         <v>33</v>
       </c>
@@ -1430,7 +1488,7 @@
       </c>
       <c r="F27" s="14"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
         <v>63</v>
       </c>
@@ -1450,7 +1508,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>41</v>
       </c>
@@ -1470,7 +1528,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
         <v>42</v>
       </c>
@@ -1490,7 +1548,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
         <v>43</v>
       </c>
@@ -1510,7 +1568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
         <v>44</v>
       </c>
@@ -1530,7 +1588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
         <v>66</v>
       </c>
@@ -1546,7 +1604,7 @@
       <c r="E33" s="9"/>
       <c r="F33" s="9"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="9"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
@@ -1554,7 +1612,7 @@
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="9"/>
       <c r="C35" s="1"/>
@@ -1562,13 +1620,13 @@
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
     </row>
-    <row r="37" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A37" s="16" t="s">
         <v>51</v>
       </c>
       <c r="B37" s="16"/>
     </row>
-    <row r="38" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
         <v>46</v>
       </c>
@@ -1584,7 +1642,7 @@
       </c>
       <c r="F38" s="8"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
         <v>37</v>
       </c>
@@ -1592,10 +1650,10 @@
         <v>55579.3</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="D39" s="11">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="E39" s="9" t="s">
         <v>63</v>
@@ -1604,7 +1662,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
         <v>45</v>
       </c>
@@ -1612,10 +1670,10 @@
         <v>1000</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D40" s="11">
-        <v>5</v>
+        <v>41</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>0</v>
       </c>
       <c r="E40" s="9" t="s">
         <v>41</v>
@@ -1624,7 +1682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
         <v>38</v>
       </c>
@@ -1632,35 +1690,35 @@
         <v>1206</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>5</v>
+        <v>42</v>
+      </c>
+      <c r="D41" s="11">
+        <v>17.5</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>42</v>
+        <v>110</v>
       </c>
       <c r="F41" s="9">
-        <v>17.5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
         <v>39</v>
       </c>
       <c r="B42" s="9">
         <v>0</v>
       </c>
-      <c r="C42" s="9"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F42" s="9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C42" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D42" s="9">
+        <v>0</v>
+      </c>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
         <v>40</v>
       </c>
@@ -1669,14 +1727,10 @@
       </c>
       <c r="C43" s="9"/>
       <c r="D43" s="11"/>
-      <c r="E43" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F43" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
         <v>63</v>
       </c>
@@ -1685,14 +1739,10 @@
       </c>
       <c r="C44" s="9"/>
       <c r="D44" s="11"/>
-      <c r="E44" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="F44" s="9">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+    </row>
+    <row r="45" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A45" s="16" t="s">
         <v>33</v>
       </c>
@@ -1710,7 +1760,7 @@
       </c>
       <c r="H45" s="16"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
         <v>63</v>
       </c>
@@ -1736,7 +1786,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
         <v>41</v>
       </c>
@@ -1762,7 +1812,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
         <v>42</v>
       </c>
@@ -1788,7 +1838,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="9" t="s">
         <v>43</v>
       </c>
@@ -1814,7 +1864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="s">
         <v>44</v>
       </c>
@@ -1840,7 +1890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="9" t="s">
         <v>66</v>
       </c>
@@ -1862,7 +1912,7 @@
       <c r="G51" s="9"/>
       <c r="H51" s="9"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="9"/>
       <c r="B52" s="9"/>
       <c r="C52" s="9"/>
@@ -1872,7 +1922,7 @@
       <c r="G52" s="9"/>
       <c r="H52" s="9"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="9"/>
       <c r="C53" s="1"/>
@@ -1892,7 +1942,7 @@
           <x14:formula1>
             <xm:f>Materials!$A$3:$A$17</xm:f>
           </x14:formula1>
-          <xm:sqref>B11 B13 D11 D13 B29 B31 D29 D31 D47 D49 B49 B47 F11 F49 F47 F29 H47 F4 F6 D41 F22 F24 D23 F40 F42 D5</xm:sqref>
+          <xm:sqref>B11 B13 D11 D13 B29 B31 D29 D31 D47 D49 B49 B47 F11 F49 F47 F29 H47 F4 F6 D22 F22 F42 D4 F24 F40 D40</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1C51B279-9347-4C56-8D0A-6867D59CEC48}">
           <x14:formula1>
@@ -1911,15 +1961,15 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -1939,7 +1989,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>8</v>
@@ -1962,7 +2012,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1989,7 +2039,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2016,7 +2066,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2040,7 +2090,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -2067,7 +2117,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -2094,7 +2144,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -2121,7 +2171,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -2148,7 +2198,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -2176,7 +2226,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -2203,7 +2253,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -2227,7 +2277,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -2254,7 +2304,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -2281,7 +2331,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -2308,7 +2358,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -2332,7 +2382,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>70</v>
       </c>
@@ -2359,12 +2409,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -2376,244 +2426,310 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18EA64E5-3D31-49CF-A28C-ED88775E3393}">
-  <dimension ref="A3:H18"/>
+  <dimension ref="A3:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.85546875" customWidth="1"/>
+    <col min="1" max="1" width="39.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.88671875" customWidth="1"/>
     <col min="5" max="5" width="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B3">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" t="s">
         <v>78</v>
       </c>
-      <c r="B4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E4" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="F4" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="G4" s="26" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E4" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" s="36">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5">
+        <f>VLOOKUP(B4,E4:F8,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="E5" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="B5">
-        <f>IF(B4="condensing",0.95,IF(B4="electric",1,0.6))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F5" s="38">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="B6">
         <v>70</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E6" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E7" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="F7" s="38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B8">
         <v>50</v>
       </c>
-      <c r="E8" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="F8" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="G8" s="28">
+      <c r="E8" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="F8" s="40">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12">
+        <f>0.008*B3</f>
+        <v>0.4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13">
+        <f>47*B3</f>
+        <v>2350</v>
+      </c>
+      <c r="C13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" s="26">
         <f>4.182</f>
         <v>4.1820000000000004</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="C15" s="26" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="26">
+        <v>998</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="26">
+        <f>Materials!E14/1000</f>
+        <v>0.49</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="E17" s="27"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" s="26">
+        <f>Materials!F14</f>
+        <v>7820</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" s="27"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" s="32">
+        <f>+B8*(PI()*((B9-2*B10)/1000)^2/4)  +  B12</f>
+        <v>0.56591536201771098</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20" s="32">
+        <f>+B8*PI()*(B9/1000)*B10/1000+B13/B18</f>
+        <v>0.35941637120621528</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="B21" s="32">
+        <f>+B19*B16</f>
+        <v>564.78353129367554</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" s="32">
+        <f>+B20*B18</f>
+        <v>2810.6360228326034</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" s="32">
+        <f>+B21*B15</f>
+        <v>2361.9247278701514</v>
+      </c>
+      <c r="C23" s="27" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="B9">
-        <v>100</v>
-      </c>
-      <c r="E9" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="F9" s="28" t="s">
-        <v>86</v>
-      </c>
-      <c r="G9" s="28">
-        <v>998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="B10">
-        <v>5</v>
-      </c>
-      <c r="E10" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="F10" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="G10" s="31">
-        <v>0.42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>87</v>
-      </c>
-      <c r="B11">
-        <v>10</v>
-      </c>
-      <c r="E11" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="F11" s="30" t="s">
-        <v>86</v>
-      </c>
-      <c r="G11" s="31">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B24" s="33">
+        <f>+B22*B17</f>
+        <v>1377.2116511879756</v>
+      </c>
+      <c r="C24" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="B12">
-        <v>0.1</v>
-      </c>
-      <c r="E12" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="F12" s="33" t="s">
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="B25" s="34">
+        <f>+B24+B23</f>
+        <v>3739.1363790581272</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="G12" s="34">
-        <f>+B8*(PI()*((B9-2*B10)/1000)^2/4)  +  B11*B12</f>
-        <v>1.3180862561759665</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>90</v>
-      </c>
-      <c r="B13">
-        <v>25</v>
-      </c>
-      <c r="E13" s="34" t="s">
+      <c r="F25" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="F13" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="G13" s="34">
-        <f>+G12*G9*G8</f>
-        <v>5501.2122498812369</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>91</v>
-      </c>
-      <c r="B14">
-        <v>4</v>
-      </c>
-      <c r="E14" s="34" t="s">
+      <c r="G25">
+        <f>B3/(B23+B24)</f>
+        <v>1.3372071765030082E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E26" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="F14" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="G14" s="34">
-        <f>+B8*PI()*(B9/1000)*B10/1000</f>
-        <v>7.8539816339744828E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>92</v>
-      </c>
-      <c r="B15">
-        <v>2</v>
-      </c>
-      <c r="E15" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="F15" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="G15">
-        <f>+G14*G11*G10</f>
-        <v>263.89378290154264</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E16" s="34" t="s">
-        <v>103</v>
-      </c>
-      <c r="F16" s="34" t="s">
-        <v>104</v>
-      </c>
-      <c r="G16">
-        <f>B3/(G13+G15)</f>
-        <v>8.6728673706397245E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E17" s="34" t="s">
-        <v>107</v>
-      </c>
-      <c r="F17" s="36">
+      <c r="F26" s="29">
         <f>+B6</f>
         <v>70</v>
       </c>
-      <c r="G17">
-        <f>70/G16/3600</f>
-        <v>2.2419856794155253</v>
-      </c>
-      <c r="H17" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="18" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E18" s="34" t="s">
-        <v>108</v>
+      <c r="G26">
+        <f>70/G25/3600</f>
+        <v>1.4541085918559384</v>
+      </c>
+      <c r="H26" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E27" s="27" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="10" type="noConversion"/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:D4" xr:uid="{8599A12F-F875-4813-B0DA-B86B0124C7AC}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:D4" xr:uid="{8599A12F-F875-4813-B0DA-B86B0124C7AC}">
       <formula1>$E$4:$G$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{F64854F5-11A9-4B68-BF19-4E028DCB28D3}">
+      <formula1>$E$4:$E$8</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed graphs, made subplot of surfaces and added hotspot plots
</commit_message>
<xml_diff>
--- a/UserInputSheet.xlsx
+++ b/UserInputSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Dads Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://abdef-my.sharepoint.com/personal/elizabeth_hemsley_formulaction_com/Documents/Documents/Python Scripts/HeatingModel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8357DFFA-50FC-42F1-ABCA-374CFBB98BAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{8357DFFA-50FC-42F1-ABCA-374CFBB98BAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85C50E39-AFC6-4FD4-B4C1-F956C4273B1C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{661BF5FC-8EDB-49B8-9F5E-EFC5E7050048}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11325" xr2:uid="{661BF5FC-8EDB-49B8-9F5E-EFC5E7050048}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="6" r:id="rId1"/>
@@ -21,6 +21,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -743,8 +754,12 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1042,23 +1057,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{776440E9-42E3-4F35-BD1F-E92FBB255ADE}">
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="12" customWidth="1"/>
-    <col min="5" max="5" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>36</v>
       </c>
@@ -1072,7 +1087,7 @@
       </c>
       <c r="I1" s="19"/>
     </row>
-    <row r="2" spans="1:10" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>46</v>
       </c>
@@ -1095,7 +1110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>37</v>
       </c>
@@ -1121,7 +1136,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>45</v>
       </c>
@@ -1150,7 +1165,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>38</v>
       </c>
@@ -1170,7 +1185,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>39</v>
       </c>
@@ -1190,7 +1205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>40</v>
       </c>
@@ -1206,7 +1221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>63</v>
       </c>
@@ -1222,7 +1237,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>33</v>
       </c>
@@ -1240,7 +1255,7 @@
       </c>
       <c r="I9" s="5"/>
     </row>
-    <row r="10" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>63</v>
       </c>
@@ -1263,7 +1278,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>41</v>
       </c>
@@ -1286,7 +1301,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>42</v>
       </c>
@@ -1309,7 +1324,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>43</v>
       </c>
@@ -1332,7 +1347,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>44</v>
       </c>
@@ -1355,7 +1370,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>66</v>
       </c>
@@ -1374,7 +1389,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -1382,7 +1397,7 @@
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="9"/>
       <c r="C17" s="1"/>
@@ -1390,13 +1405,13 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
         <v>49</v>
       </c>
       <c r="B19" s="14"/>
     </row>
-    <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>46</v>
       </c>
@@ -1413,7 +1428,7 @@
       </c>
       <c r="F20" s="8"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>37</v>
       </c>
@@ -1430,10 +1445,10 @@
         <v>63</v>
       </c>
       <c r="F21" s="11">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>45</v>
       </c>
@@ -1453,7 +1468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>38</v>
       </c>
@@ -1473,7 +1488,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>39</v>
       </c>
@@ -1493,7 +1508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>40</v>
       </c>
@@ -1509,7 +1524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>62</v>
       </c>
@@ -1522,10 +1537,10 @@
         <v>111</v>
       </c>
       <c r="F26" s="9">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="14" t="s">
         <v>33</v>
       </c>
@@ -1539,7 +1554,7 @@
       </c>
       <c r="F27" s="14"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>63</v>
       </c>
@@ -1559,7 +1574,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>41</v>
       </c>
@@ -1579,7 +1594,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>42</v>
       </c>
@@ -1599,7 +1614,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>43</v>
       </c>
@@ -1619,7 +1634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>44</v>
       </c>
@@ -1639,7 +1654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>66</v>
       </c>
@@ -1655,7 +1670,7 @@
       <c r="E33" s="9"/>
       <c r="F33" s="9"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="9"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
@@ -1663,7 +1678,7 @@
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="9"/>
       <c r="C35" s="1"/>
@@ -1671,13 +1686,13 @@
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
     </row>
-    <row r="37" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A37" s="16" t="s">
         <v>51</v>
       </c>
       <c r="B37" s="16"/>
     </row>
-    <row r="38" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
         <v>46</v>
       </c>
@@ -1694,7 +1709,7 @@
       </c>
       <c r="F38" s="8"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>37</v>
       </c>
@@ -1711,10 +1726,10 @@
         <v>63</v>
       </c>
       <c r="F39" s="11">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>45</v>
       </c>
@@ -1734,7 +1749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>38</v>
       </c>
@@ -1754,7 +1769,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>39</v>
       </c>
@@ -1774,7 +1789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>40</v>
       </c>
@@ -1790,7 +1805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>63</v>
       </c>
@@ -1806,7 +1821,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A45" s="16" t="s">
         <v>33</v>
       </c>
@@ -1824,7 +1839,7 @@
       </c>
       <c r="H45" s="16"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>63</v>
       </c>
@@ -1850,7 +1865,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>41</v>
       </c>
@@ -1876,7 +1891,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>42</v>
       </c>
@@ -1902,7 +1917,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>43</v>
       </c>
@@ -1928,7 +1943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>44</v>
       </c>
@@ -1954,7 +1969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>66</v>
       </c>
@@ -1976,7 +1991,7 @@
       <c r="G51" s="9"/>
       <c r="H51" s="9"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="9"/>
       <c r="B52" s="9"/>
       <c r="C52" s="9"/>
@@ -1986,7 +2001,7 @@
       <c r="G52" s="9"/>
       <c r="H52" s="9"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="9"/>
       <c r="C53" s="1"/>
@@ -2028,12 +2043,12 @@
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -2053,7 +2068,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>8</v>
@@ -2076,7 +2091,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2103,7 +2118,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2130,7 +2145,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2154,7 +2169,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -2181,7 +2196,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -2208,7 +2223,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -2235,7 +2250,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -2262,7 +2277,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -2290,7 +2305,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -2317,7 +2332,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -2341,7 +2356,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -2368,7 +2383,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -2395,7 +2410,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -2422,7 +2437,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -2446,7 +2461,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>70</v>
       </c>
@@ -2473,12 +2488,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -2496,17 +2511,17 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.33203125" customWidth="1"/>
+    <col min="1" max="1" width="39.28515625" customWidth="1"/>
     <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.88671875" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.85546875" customWidth="1"/>
     <col min="5" max="5" width="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.6640625" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -2514,7 +2529,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>107</v>
       </c>
@@ -2528,7 +2543,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -2543,7 +2558,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>97</v>
       </c>
@@ -2557,7 +2572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E7" s="37" t="s">
         <v>108</v>
       </c>
@@ -2565,7 +2580,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>84</v>
       </c>
@@ -2579,7 +2594,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>85</v>
       </c>
@@ -2587,7 +2602,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
         <v>92</v>
       </c>
@@ -2595,7 +2610,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>102</v>
       </c>
@@ -2607,7 +2622,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>103</v>
       </c>
@@ -2619,7 +2634,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
         <v>79</v>
       </c>
@@ -2631,7 +2646,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
         <v>80</v>
       </c>
@@ -2642,7 +2657,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="26" t="s">
         <v>81</v>
       </c>
@@ -2655,7 +2670,7 @@
       </c>
       <c r="E17" s="27"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
         <v>82</v>
       </c>
@@ -2668,7 +2683,7 @@
       </c>
       <c r="E18" s="27"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
         <v>91</v>
       </c>
@@ -2680,7 +2695,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
         <v>90</v>
       </c>
@@ -2692,7 +2707,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
         <v>105</v>
       </c>
@@ -2704,7 +2719,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
         <v>106</v>
       </c>
@@ -2716,7 +2731,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
         <v>87</v>
       </c>
@@ -2728,7 +2743,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
         <v>93</v>
       </c>
@@ -2740,7 +2755,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
         <v>101</v>
       </c>
@@ -2762,7 +2777,7 @@
         <v>1.3372071765030082E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E26" s="27" t="s">
         <v>98</v>
       </c>
@@ -2778,7 +2793,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E27" s="27" t="s">
         <v>99</v>
       </c>

</xml_diff>

<commit_message>
added plots to show internal temperature of surfaces + internals for given time array
</commit_message>
<xml_diff>
--- a/UserInputSheet.xlsx
+++ b/UserInputSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Dads Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED88976-865B-4EFC-8DAA-7DF318595DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D37CC5-C467-4E12-9FEA-82ACD81FDDB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{661BF5FC-8EDB-49B8-9F5E-EFC5E7050048}"/>
   </bookViews>
@@ -1050,8 +1050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{776440E9-42E3-4F35-BD1F-E92FBB255ADE}">
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1139,7 +1139,7 @@
         <v>41</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>41</v>
@@ -1168,7 +1168,7 @@
         <v>42</v>
       </c>
       <c r="D5" s="11">
-        <v>0.5</v>
+        <v>17.5</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
add heater on/off and turned of hotspots when heaters off
</commit_message>
<xml_diff>
--- a/UserInputSheet.xlsx
+++ b/UserInputSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Dads Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D37CC5-C467-4E12-9FEA-82ACD81FDDB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3B80CB-FD17-440F-BFBF-B5E990BCDB62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{661BF5FC-8EDB-49B8-9F5E-EFC5E7050048}"/>
+    <workbookView xWindow="-28920" yWindow="-3750" windowWidth="29040" windowHeight="15840" xr2:uid="{661BF5FC-8EDB-49B8-9F5E-EFC5E7050048}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="118">
   <si>
     <t>Brick</t>
   </si>
@@ -437,6 +437,9 @@
   </si>
   <si>
     <t>iloc[7-14]</t>
+  </si>
+  <si>
+    <t>Underfloor Heating</t>
   </si>
 </sst>
 </file>
@@ -672,7 +675,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -730,6 +733,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1050,8 +1054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{776440E9-42E3-4F35-BD1F-E92FBB255ADE}">
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1062,7 +1066,7 @@
     <col min="4" max="4" width="11.5546875" style="12" customWidth="1"/>
     <col min="5" max="5" width="29.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1084,8 +1088,9 @@
       <c r="A2" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="9">
-        <v>0</v>
+      <c r="B2" s="43">
+        <f ca="1">I2</f>
+        <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>73</v>
@@ -1098,8 +1103,8 @@
       <c r="H2" t="s">
         <v>61</v>
       </c>
-      <c r="I2">
-        <v>0</v>
+      <c r="I2" s="31">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1410,9 +1415,9 @@
       <c r="A20" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="9">
-        <f>B2</f>
-        <v>0</v>
+      <c r="B20" s="43">
+        <f ca="1">I2</f>
+        <v>5</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>73</v>
@@ -1691,9 +1696,9 @@
       <c r="A38" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B38" s="9">
-        <f>B2</f>
-        <v>0</v>
+      <c r="B38" s="43">
+        <f ca="1">I2</f>
+        <v>5</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>73</v>
@@ -1703,6 +1708,10 @@
         <v>74</v>
       </c>
       <c r="F38" s="8"/>
+      <c r="G38" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="H38" s="8"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
@@ -1723,6 +1732,12 @@
       <c r="F39" s="11">
         <v>0.01</v>
       </c>
+      <c r="G39" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H39" s="11">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
@@ -1743,6 +1758,12 @@
       <c r="F40" s="9" t="s">
         <v>0</v>
       </c>
+      <c r="G40" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H40" s="9" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
@@ -1763,6 +1784,12 @@
       <c r="F41" s="11">
         <v>17.5</v>
       </c>
+      <c r="G41" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H41" s="11">
+        <v>17.5</v>
+      </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
@@ -1782,6 +1809,12 @@
       </c>
       <c r="F42" s="9" t="s">
         <v>0</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H42" s="9" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
@@ -1799,6 +1832,12 @@
       <c r="F43" s="11">
         <v>0</v>
       </c>
+      <c r="G43" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H43" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
@@ -1813,6 +1852,12 @@
         <v>111</v>
       </c>
       <c r="F44" s="9">
+        <v>50</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="H44" s="9">
         <v>50</v>
       </c>
     </row>
@@ -2016,7 +2061,7 @@
           <x14:formula1>
             <xm:f>Materials!$A$3:$A$17</xm:f>
           </x14:formula1>
-          <xm:sqref>B11 B13 D11 D13 B29 B31 D29 D31 D47 D49 B49 B47 F11 F49 F47 F29 H47 F22 F24 D22 F4 F6 D4 D40 F40 F42</xm:sqref>
+          <xm:sqref>B11 B13 D11 D13 B29 B31 D29 D31 D47 D49 B49 B47 F11 F49 F47 F29 H47 F22 F24 D22 F4 F6 D4 D40 F40 F42 H40 H42</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1C51B279-9347-4C56-8D0A-6867D59CEC48}">
           <x14:formula1>

</xml_diff>